<commit_message>
Att Média e Estatística Descritiva no DT
</commit_message>
<xml_diff>
--- a/Kabum/new_excel.xlsx
+++ b/Kabum/new_excel.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Desktop\Projetos GIT pessoal\Project-Kabum\Kabum\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4E2B10-6748-4D53-AF85-7E314F33E9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -40,11 +34,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,13 +45,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -100,36 +84,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -171,7 +144,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -203,27 +176,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -255,24 +210,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -448,20 +385,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="104.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,139 +400,139 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>3074.15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>1907.99</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>2682.59</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>3999.99</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>2825.85</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>3899.99</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <v>1999.99</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9">
         <v>3100.24</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="2">
-        <v>2499.9899999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>2499.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11">
         <v>1599.99</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12">
         <v>2899.99</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13">
         <v>3999.99</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14">
         <v>3499.99</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15">
         <v>3024.9</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16">
         <v>3899.99</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17">
         <v>3199.99</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18">
         <v>3799.99</v>
       </c>
     </row>

</xml_diff>